<commit_message>
edit the dataset 1
</commit_message>
<xml_diff>
--- a/Copy of Beach Work HTMLversion.xlsx
+++ b/Copy of Beach Work HTMLversion.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -257,15 +257,9 @@
     <t>Bank B</t>
   </si>
   <si>
-    <t>London</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
-    <t>Stockholm</t>
-  </si>
-  <si>
     <t>France</t>
   </si>
   <si>
@@ -275,22 +269,22 @@
     <t>Spain</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>Denmark</t>
   </si>
   <si>
     <t>Finland</t>
   </si>
   <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
     <t>Russia</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">united states of america </t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1029,7 @@
   <dimension ref="B1:N51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1043,7 +1037,7 @@
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" customWidth="1"/>
@@ -1103,7 +1097,7 @@
         <v>56</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="22" t="s">
@@ -1121,7 +1115,7 @@
       </c>
       <c r="K2" s="12">
         <f t="shared" ref="K2:K30" ca="1" si="0">IF(COUNTA(J2)=1,IF(ISERROR(J2-TODAY()),"Deadline missing",IF(J2-TODAY()&lt;0,"Past deadline",IF(J2-TODAY()=0,"Due today",J2-TODAY()))),"")</f>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L2" s="8" t="str">
         <f t="shared" ref="L2:L30" ca="1" si="1">IF(OR(D:D="HOL",D:D="Pat L"),"On holiday",IF(C:C="No","",IF(OR(K2="Past deadline",K2="Deadline missing"),"Unassigned","Ongoing")))</f>
@@ -1138,7 +1132,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="22" t="s">
@@ -1156,7 +1150,7 @@
       </c>
       <c r="K3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L3" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1173,7 +1167,7 @@
         <v>56</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="22" t="s">
@@ -1191,7 +1185,7 @@
       </c>
       <c r="K4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L4" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1208,7 +1202,7 @@
         <v>57</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="22" t="s">
@@ -1226,7 +1220,7 @@
       </c>
       <c r="K5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L5" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1243,7 +1237,7 @@
         <v>56</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E6" s="25"/>
       <c r="F6" s="22" t="s">
@@ -1261,7 +1255,7 @@
       </c>
       <c r="K6" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L6" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1277,7 +1271,7 @@
         <v>57</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="22" t="s">
@@ -1295,7 +1289,7 @@
       </c>
       <c r="K7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="L7" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1311,7 +1305,7 @@
         <v>56</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="22" t="s">
@@ -1329,7 +1323,7 @@
       </c>
       <c r="K8" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L8" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1345,7 +1339,7 @@
         <v>57</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E9" s="28"/>
       <c r="F9" s="22" t="s">
@@ -1363,7 +1357,7 @@
       </c>
       <c r="K9" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L9" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1379,7 +1373,7 @@
         <v>56</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="22" t="s">
@@ -1397,7 +1391,7 @@
       </c>
       <c r="K10" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L10" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1413,7 +1407,7 @@
         <v>57</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="22" t="s">
@@ -1431,7 +1425,7 @@
       </c>
       <c r="K11" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L11" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1447,7 +1441,7 @@
         <v>56</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E12" s="25"/>
       <c r="F12" s="22" t="s">
@@ -1465,7 +1459,7 @@
       </c>
       <c r="K12" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L12" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1481,7 +1475,7 @@
         <v>57</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="22" t="s">
@@ -1499,7 +1493,7 @@
       </c>
       <c r="K13" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L13" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1515,7 +1509,7 @@
         <v>56</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="22" t="s">
@@ -1533,7 +1527,7 @@
       </c>
       <c r="K14" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L14" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1549,7 +1543,7 @@
         <v>57</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="22" t="s">
@@ -1567,7 +1561,7 @@
       </c>
       <c r="K15" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L15" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1583,7 +1577,7 @@
         <v>56</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="22" t="s">
@@ -1601,7 +1595,7 @@
       </c>
       <c r="K16" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L16" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1617,7 +1611,7 @@
         <v>57</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E17" s="25"/>
       <c r="F17" s="22" t="s">
@@ -1635,7 +1629,7 @@
       </c>
       <c r="K17" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L17" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1651,7 +1645,7 @@
         <v>56</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="22" t="s">
@@ -1669,7 +1663,7 @@
       </c>
       <c r="K18" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L18" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1685,7 +1679,7 @@
         <v>57</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E19" s="25"/>
       <c r="F19" s="22" t="s">
@@ -1703,7 +1697,7 @@
       </c>
       <c r="K19" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L19" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1719,7 +1713,7 @@
         <v>56</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="22" t="s">
@@ -1737,7 +1731,7 @@
       </c>
       <c r="K20" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L20" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1753,7 +1747,7 @@
         <v>57</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="22" t="s">
@@ -1771,7 +1765,7 @@
       </c>
       <c r="K21" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L21" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1787,7 +1781,7 @@
         <v>56</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E22" s="25"/>
       <c r="F22" s="22" t="s">
@@ -1805,7 +1799,7 @@
       </c>
       <c r="K22" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L22" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1821,7 +1815,7 @@
         <v>57</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E23" s="25"/>
       <c r="F23" s="22" t="s">
@@ -1839,7 +1833,7 @@
       </c>
       <c r="K23" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L23" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1855,7 +1849,7 @@
         <v>56</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E24" s="23"/>
       <c r="F24" s="22" t="s">
@@ -1873,7 +1867,7 @@
       </c>
       <c r="K24" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L24" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1889,7 +1883,7 @@
         <v>57</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E25" s="25"/>
       <c r="F25" s="22" t="s">
@@ -1907,7 +1901,7 @@
       </c>
       <c r="K25" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L25" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1923,7 +1917,7 @@
         <v>56</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E26" s="25"/>
       <c r="F26" s="22" t="s">
@@ -1941,7 +1935,7 @@
       </c>
       <c r="K26" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L26" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -1957,7 +1951,7 @@
         <v>57</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="22" t="s">
@@ -1975,7 +1969,7 @@
       </c>
       <c r="K27" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L27" s="8" t="str">
         <f t="shared" si="1"/>
@@ -1991,7 +1985,7 @@
         <v>56</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E28" s="28"/>
       <c r="F28" s="22" t="s">
@@ -2009,7 +2003,7 @@
       </c>
       <c r="K28" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L28" s="8" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2025,7 +2019,7 @@
         <v>57</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E29" s="25"/>
       <c r="F29" s="22" t="s">
@@ -2043,7 +2037,7 @@
       </c>
       <c r="K29" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L29" s="8" t="str">
         <f t="shared" si="1"/>
@@ -2059,7 +2053,7 @@
         <v>56</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="22" t="s">
@@ -2077,7 +2071,7 @@
       </c>
       <c r="K30" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="L30" s="8" t="str">
         <f t="shared" ca="1" si="1"/>

</xml_diff>

<commit_message>
edit the dataset 2
</commit_message>
<xml_diff>
--- a/Copy of Beach Work HTMLversion.xlsx
+++ b/Copy of Beach Work HTMLversion.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -284,7 +284,10 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t xml:space="preserve">united states of america </t>
+    <t>united states</t>
+  </si>
+  <si>
+    <t xml:space="preserve">united states </t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1032,7 @@
   <dimension ref="B1:N51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1645,7 +1648,7 @@
         <v>56</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="22" t="s">
@@ -1985,7 +1988,7 @@
         <v>56</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E28" s="28"/>
       <c r="F28" s="22" t="s">

</xml_diff>

<commit_message>
edit the dataset 3
</commit_message>
<xml_diff>
--- a/Copy of Beach Work HTMLversion.xlsx
+++ b/Copy of Beach Work HTMLversion.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -284,10 +284,7 @@
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>united states</t>
-  </si>
-  <si>
-    <t xml:space="preserve">united states </t>
+    <t>United States</t>
   </si>
 </sst>
 </file>
@@ -1648,7 +1645,7 @@
         <v>56</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E18" s="25"/>
       <c r="F18" s="22" t="s">
@@ -1988,7 +1985,7 @@
         <v>56</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E28" s="28"/>
       <c r="F28" s="22" t="s">

</xml_diff>